<commit_message>
ajout TOP rapport dose abs
</commit_message>
<xml_diff>
--- a/RT3/mesures/export_excel/champ_3x3.xlsx
+++ b/RT3/mesures/export_excel/champ_3x3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/LEXAR/Fiches_DQ/RT/RT3/mesures/export_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE85926-9164-E846-A7EC-A72C57EC207A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA49AAF3-D4FA-EE4A-A01F-AB797048C0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Crossline X6 Ouverture" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
   <si>
     <t xml:space="preserve"> Crossline</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t> Ratio</t>
+  </si>
+  <si>
+    <t> Crossline</t>
   </si>
 </sst>
 </file>
@@ -1304,9 +1307,7 @@
   </sheetPr>
   <dimension ref="A1:B259"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3387,682 +3388,682 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEF1F6F-AA56-8B49-BF05-40ED04465699}">
   <dimension ref="A1:B84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="9">
+        <v>50</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="9">
+        <v>49</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>47.2</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>45.8</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
+        <v>44.7</v>
+      </c>
+      <c r="B6" s="9">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
+        <v>43.5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
+        <v>42.4</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
+        <v>41.3</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="9">
+        <v>40</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="9">
+        <v>37.5</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
+        <v>36.4</v>
+      </c>
+      <c r="B13" s="9">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
+        <v>35.1</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
+        <v>33.9</v>
+      </c>
+      <c r="B15" s="9">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="B16" s="9">
+        <v>3.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" s="9">
+        <v>31.5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" s="9">
+        <v>30.3</v>
+      </c>
+      <c r="B18" s="9">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" s="9">
+        <v>29.1</v>
+      </c>
+      <c r="B19" s="9">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" s="9">
+        <v>27.9</v>
+      </c>
+      <c r="B20" s="9">
+        <v>4.6500000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" s="9">
+        <v>26.6</v>
+      </c>
+      <c r="B21" s="9">
+        <v>5.09</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" s="9">
+        <v>25.5</v>
+      </c>
+      <c r="B22" s="9">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="9">
+        <v>24.3</v>
+      </c>
+      <c r="B23" s="9">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" s="9">
+        <v>23.1</v>
+      </c>
+      <c r="B24" s="9">
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" s="9">
+        <v>21.8</v>
+      </c>
+      <c r="B25" s="9">
+        <v>10.28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" s="9">
+        <v>20.6</v>
+      </c>
+      <c r="B26" s="9">
+        <v>14.96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" s="9">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="B27" s="9">
+        <v>23.31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A28" s="9">
+        <v>18.2</v>
+      </c>
+      <c r="B28" s="9">
+        <v>35.159999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" s="9">
+        <v>17</v>
+      </c>
+      <c r="B29" s="9">
+        <v>49.42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" s="9">
+        <v>15.8</v>
+      </c>
+      <c r="B30" s="9">
+        <v>64.349999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" s="9">
+        <v>14.6</v>
+      </c>
+      <c r="B31" s="9">
+        <v>77.64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A32" s="9">
+        <v>13.4</v>
+      </c>
+      <c r="B32" s="9">
+        <v>87.85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A33" s="9">
+        <v>12.2</v>
+      </c>
+      <c r="B33" s="9">
+        <v>93.39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A34" s="9">
+        <v>11</v>
+      </c>
+      <c r="B34" s="9">
+        <v>96.13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A35" s="9">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="B35" s="9">
+        <v>97.92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A36" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="B36" s="9">
+        <v>98.53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A37" s="9">
+        <v>7.3</v>
+      </c>
+      <c r="B37" s="9">
+        <v>99.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A38" s="9">
+        <v>6.1</v>
+      </c>
+      <c r="B38" s="9">
+        <v>99.57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A39" s="9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B39" s="9">
+        <v>99.59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A40" s="9">
+        <v>3.7</v>
+      </c>
+      <c r="B40" s="9">
+        <v>99.61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A41" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="B41" s="9">
+        <v>99.74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A42" s="9">
+        <v>1.3</v>
+      </c>
+      <c r="B42" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A43" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="B43" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A44" s="9">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="B44" s="9">
+        <v>99.74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A45" s="9">
+        <v>-2.4</v>
+      </c>
+      <c r="B45" s="9">
+        <v>99.99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A46" s="9">
+        <v>-3.6</v>
+      </c>
+      <c r="B46" s="9">
+        <v>99.76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A47" s="9">
+        <v>-4.8</v>
+      </c>
+      <c r="B47" s="9">
+        <v>99.44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A48" s="9">
+        <v>-6</v>
+      </c>
+      <c r="B48" s="9">
+        <v>99.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" s="9">
+        <v>-7.2</v>
+      </c>
+      <c r="B49" s="9">
+        <v>98.94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A50" s="9">
+        <v>-8.4</v>
+      </c>
+      <c r="B50" s="9">
+        <v>98.63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" s="9">
+        <v>-9.6</v>
+      </c>
+      <c r="B51" s="9">
+        <v>97.72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" s="9">
+        <v>-10.8</v>
+      </c>
+      <c r="B52" s="9">
+        <v>95.92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" s="9">
+        <v>-12</v>
+      </c>
+      <c r="B53" s="9">
+        <v>92.69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" s="9">
+        <v>-13.2</v>
+      </c>
+      <c r="B54" s="9">
+        <v>85.78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" s="9">
+        <v>-14.4</v>
+      </c>
+      <c r="B55" s="9">
+        <v>75.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" s="9">
+        <v>-15.7</v>
+      </c>
+      <c r="B56" s="9">
+        <v>61.88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" s="9">
+        <v>-16.8</v>
+      </c>
+      <c r="B57" s="9">
+        <v>47.41</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" s="9">
+        <v>-18.100000000000001</v>
+      </c>
+      <c r="B58" s="9">
+        <v>33.340000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" s="9">
+        <v>-19.3</v>
+      </c>
+      <c r="B59" s="9">
+        <v>21.48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" s="9">
+        <v>-20.5</v>
+      </c>
+      <c r="B60" s="9">
+        <v>13.91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" s="9">
+        <v>-21.7</v>
+      </c>
+      <c r="B61" s="9">
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" s="9">
+        <v>-22.9</v>
+      </c>
+      <c r="B62" s="9">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" s="9">
+        <v>-24.1</v>
+      </c>
+      <c r="B63" s="9">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" s="9">
+        <v>-25.3</v>
+      </c>
+      <c r="B64" s="9">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" s="9">
+        <v>-26.6</v>
+      </c>
+      <c r="B65" s="9">
+        <v>4.93</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" s="9">
+        <v>-27.7</v>
+      </c>
+      <c r="B66" s="9">
+        <v>4.5599999999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" s="9">
+        <v>-28.9</v>
+      </c>
+      <c r="B67" s="9">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" s="9">
+        <v>-30.2</v>
+      </c>
+      <c r="B68" s="9">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" s="9">
+        <v>-31.3</v>
+      </c>
+      <c r="B69" s="9">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" s="9">
+        <v>-32.6</v>
+      </c>
+      <c r="B70" s="9">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" s="9">
+        <v>-33.799999999999997</v>
+      </c>
+      <c r="B71" s="9">
+        <v>3.27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" s="9">
+        <v>-34.9</v>
+      </c>
+      <c r="B72" s="9">
+        <v>3.12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" s="9">
+        <v>-36.200000000000003</v>
+      </c>
+      <c r="B73" s="9">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" s="9">
+        <v>-37.4</v>
+      </c>
+      <c r="B74" s="9">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" s="9">
+        <v>-38.6</v>
+      </c>
+      <c r="B75" s="9">
+        <v>2.69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" s="9">
+        <v>-39.799999999999997</v>
+      </c>
+      <c r="B76" s="9">
+        <v>2.58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" s="9">
+        <v>-41.1</v>
+      </c>
+      <c r="B77" s="9">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" s="9">
+        <v>-42.2</v>
+      </c>
+      <c r="B78" s="9">
+        <v>2.3199999999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" s="9">
+        <v>-43.5</v>
+      </c>
+      <c r="B79" s="9">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" s="9">
+        <v>-44.7</v>
+      </c>
+      <c r="B80" s="9">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" s="9">
+        <v>-45.8</v>
+      </c>
+      <c r="B81" s="9">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A82" s="9">
+        <v>-47</v>
+      </c>
+      <c r="B82" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="6">
-        <v>50</v>
-      </c>
-      <c r="B2" s="6">
-        <v>1.63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="6">
-        <v>49</v>
-      </c>
-      <c r="B3" s="6">
-        <v>1.39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="8">
-        <v>47.2</v>
-      </c>
-      <c r="B4" s="6">
-        <v>1.46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="8">
-        <v>45.8</v>
-      </c>
-      <c r="B5" s="8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="8">
-        <v>44.7</v>
-      </c>
-      <c r="B6" s="6">
-        <v>1.61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="8">
-        <v>43.5</v>
-      </c>
-      <c r="B7" s="6">
-        <v>1.71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="8">
-        <v>42.4</v>
-      </c>
-      <c r="B8" s="6">
-        <v>1.77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="8">
-        <v>41.3</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="6">
-        <v>40</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1.93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="8">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="B11" s="6">
-        <v>2.0699999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="8">
-        <v>37.5</v>
-      </c>
-      <c r="B12" s="8">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="8">
-        <v>36.4</v>
-      </c>
-      <c r="B13" s="6">
-        <v>2.27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="8">
-        <v>35.1</v>
-      </c>
-      <c r="B14" s="6">
-        <v>2.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="8">
-        <v>33.9</v>
-      </c>
-      <c r="B15" s="6">
-        <v>2.48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="8">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="B16" s="8">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17" s="8">
-        <v>31.5</v>
-      </c>
-      <c r="B17" s="6">
-        <v>2.74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18" s="8">
-        <v>30.3</v>
-      </c>
-      <c r="B18" s="6">
-        <v>2.96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19" s="8">
-        <v>29.1</v>
-      </c>
-      <c r="B19" s="6">
-        <v>3.11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20" s="8">
-        <v>27.9</v>
-      </c>
-      <c r="B20" s="6">
-        <v>3.47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21" s="8">
-        <v>26.6</v>
-      </c>
-      <c r="B21" s="6">
-        <v>3.79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22" s="8">
-        <v>25.5</v>
-      </c>
-      <c r="B22" s="6">
-        <v>4.24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23" s="8">
-        <v>24.3</v>
-      </c>
-      <c r="B23" s="6">
-        <v>4.83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24" s="8">
-        <v>23.1</v>
-      </c>
-      <c r="B24" s="6">
-        <v>5.93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25" s="8">
-        <v>21.8</v>
-      </c>
-      <c r="B25" s="6">
-        <v>7.58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26" s="8">
-        <v>20.6</v>
-      </c>
-      <c r="B26" s="6">
-        <v>11.04</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27" s="8">
-        <v>19.399999999999999</v>
-      </c>
-      <c r="B27" s="6">
-        <v>17.29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28" s="8">
-        <v>18.2</v>
-      </c>
-      <c r="B28" s="6">
-        <v>26.13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29" s="6">
-        <v>17</v>
-      </c>
-      <c r="B29" s="6">
-        <v>36.82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30" s="8">
-        <v>15.8</v>
-      </c>
-      <c r="B30" s="6">
-        <v>48.04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31" s="8">
-        <v>14.6</v>
-      </c>
-      <c r="B31" s="6">
-        <v>57.92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32" s="8">
-        <v>13.4</v>
-      </c>
-      <c r="B32" s="6">
-        <v>65.61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33" s="8">
-        <v>12.2</v>
-      </c>
-      <c r="B33" s="6">
-        <v>69.680000000000007</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34" s="6">
-        <v>11</v>
-      </c>
-      <c r="B34" s="6">
-        <v>71.67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35" s="8">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="B35" s="6">
-        <v>73.010000000000005</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36" s="8">
-        <v>8.5</v>
-      </c>
-      <c r="B36" s="6">
-        <v>73.430000000000007</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37" s="8">
-        <v>7.3</v>
-      </c>
-      <c r="B37" s="6">
-        <v>73.86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38" s="8">
-        <v>6.1</v>
-      </c>
-      <c r="B38" s="6">
-        <v>74.23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39" s="8">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="B39" s="6">
-        <v>74.22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A40" s="8">
-        <v>3.7</v>
-      </c>
-      <c r="B40" s="6">
-        <v>74.23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A41" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="B41" s="6">
-        <v>74.33</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A42" s="8">
-        <v>1.3</v>
-      </c>
-      <c r="B42" s="6">
-        <v>74.540000000000006</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A43" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="B43" s="6">
-        <v>74.540000000000006</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A44" s="8">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="B44" s="6">
-        <v>74.319999999999993</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A45" s="8">
-        <v>-2.4</v>
-      </c>
-      <c r="B45" s="6">
-        <v>74.53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A46" s="8">
-        <v>-3.6</v>
-      </c>
-      <c r="B46" s="6">
-        <v>74.36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A47" s="8">
-        <v>-4.8</v>
-      </c>
-      <c r="B47" s="6">
-        <v>74.11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A48" s="6">
-        <v>-6</v>
-      </c>
-      <c r="B48" s="6">
-        <v>73.930000000000007</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A49" s="8">
-        <v>-7.2</v>
-      </c>
-      <c r="B49" s="6">
-        <v>73.739999999999995</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A50" s="8">
-        <v>-8.4</v>
-      </c>
-      <c r="B50" s="6">
-        <v>73.52</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A51" s="8">
-        <v>-9.6</v>
-      </c>
-      <c r="B51" s="6">
-        <v>72.86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A52" s="8">
-        <v>-10.8</v>
-      </c>
-      <c r="B52" s="6">
-        <v>71.52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A53" s="6">
-        <v>-12</v>
-      </c>
-      <c r="B53" s="6">
-        <v>69.16</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A54" s="8">
-        <v>-13.2</v>
-      </c>
-      <c r="B54" s="6">
-        <v>64.06</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A55" s="8">
-        <v>-14.4</v>
-      </c>
-      <c r="B55" s="8">
-        <v>56.2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A56" s="8">
-        <v>-15.7</v>
-      </c>
-      <c r="B56" s="6">
-        <v>46.19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A57" s="8">
-        <v>-16.8</v>
-      </c>
-      <c r="B57" s="6">
-        <v>35.29</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A58" s="8">
-        <v>-18.100000000000001</v>
-      </c>
-      <c r="B58" s="6">
-        <v>24.77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A59" s="8">
-        <v>-19.3</v>
-      </c>
-      <c r="B59" s="6">
-        <v>15.88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A60" s="8">
-        <v>-20.5</v>
-      </c>
-      <c r="B60" s="6">
-        <v>10.23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A61" s="8">
-        <v>-21.7</v>
-      </c>
-      <c r="B61" s="6">
-        <v>7.27</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A62" s="8">
-        <v>-22.9</v>
-      </c>
-      <c r="B62" s="6">
-        <v>5.63</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A63" s="8">
-        <v>-24.1</v>
-      </c>
-      <c r="B63" s="8">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A64" s="8">
-        <v>-25.3</v>
-      </c>
-      <c r="B64" s="8">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A65" s="8">
-        <v>-26.6</v>
-      </c>
-      <c r="B65" s="6">
-        <v>3.67</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A66" s="8">
-        <v>-27.7</v>
-      </c>
-      <c r="B66" s="6">
-        <v>3.39</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A67" s="8">
-        <v>-28.9</v>
-      </c>
-      <c r="B67" s="6">
-        <v>3.16</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A68" s="8">
-        <v>-30.2</v>
-      </c>
-      <c r="B68" s="6">
-        <v>2.95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A69" s="8">
-        <v>-31.3</v>
-      </c>
-      <c r="B69" s="8">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A70" s="8">
-        <v>-32.6</v>
-      </c>
-      <c r="B70" s="6">
-        <v>2.57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A71" s="8">
-        <v>-33.799999999999997</v>
-      </c>
-      <c r="B71" s="6">
-        <v>2.4300000000000002</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A72" s="8">
-        <v>-34.9</v>
-      </c>
-      <c r="B72" s="6">
-        <v>2.3199999999999998</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A73" s="8">
-        <v>-36.200000000000003</v>
-      </c>
-      <c r="B73" s="6">
-        <v>2.19</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A74" s="8">
-        <v>-37.4</v>
-      </c>
-      <c r="B74" s="6">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A75" s="8">
-        <v>-38.6</v>
-      </c>
-      <c r="B75" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A76" s="8">
-        <v>-39.799999999999997</v>
-      </c>
-      <c r="B76" s="6">
-        <v>1.92</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A77" s="8">
-        <v>-41.1</v>
-      </c>
-      <c r="B77" s="6">
-        <v>1.79</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A78" s="8">
-        <v>-42.2</v>
-      </c>
-      <c r="B78" s="6">
-        <v>1.73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A79" s="8">
-        <v>-43.5</v>
-      </c>
-      <c r="B79" s="6">
-        <v>1.71</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A80" s="8">
-        <v>-44.7</v>
-      </c>
-      <c r="B80" s="6">
-        <v>1.66</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A81" s="8">
-        <v>-45.8</v>
-      </c>
-      <c r="B81" s="6">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A82" s="6">
-        <v>-47</v>
-      </c>
-      <c r="B82" s="6">
-        <v>1.49</v>
-      </c>
-    </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A83" s="8">
+      <c r="A83" s="9">
         <v>-48.3</v>
       </c>
-      <c r="B83" s="6">
-        <v>1.42</v>
+      <c r="B83" s="9">
+        <v>1.91</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A84" s="8">
+      <c r="A84" s="9">
         <v>-50.3</v>
       </c>
-      <c r="B84" s="6">
-        <v>1.36</v>
+      <c r="B84" s="9">
+        <v>1.82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>